<commit_message>
SPRINT C - DESIGN - UCD and DM updated -  Information Updates on both - Improved UCD overall organization.
</commit_message>
<xml_diff>
--- a/docs/SprintC/assessmentGridLAPR2_Class1DA_TeamG02.xlsx
+++ b/docs/SprintC/assessmentGridLAPR2_Class1DA_TeamG02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guga\OneDrive\Documentos\lei-22-s2-1da-g02\docs\SprintC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0520D17B-3A88-4ED6-B432-0808697E8AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846FB104-EA0F-4F64-9F76-BB5DB5B80E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="94">
   <si>
     <t>Evaluation</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>Total (0-20)</t>
+  </si>
+  <si>
+    <t>1DA</t>
+  </si>
+  <si>
+    <t>G02 - Backloggers</t>
   </si>
 </sst>
 </file>
@@ -668,25 +674,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1201,7 +1207,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,11 +1231,11 @@
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
       <c r="H2" t="s">
         <v>15</v>
       </c>
@@ -1238,29 +1244,33 @@
       <c r="A3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="I3" s="43" t="s">
+      <c r="B3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="43"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="11">
         <f>F5</f>
         <v>1210816</v>
@@ -1343,11 +1353,11 @@
       <c r="N6" s="12"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
       <c r="E7" s="10" t="s">
         <v>28</v>
       </c>
@@ -1438,10 +1448,10 @@
       <c r="F10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="41" t="s">
+      <c r="G10" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="41"/>
+      <c r="H10" s="43"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -1450,11 +1460,11 @@
       <c r="N10" s="12"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
       <c r="I12" t="s">
         <v>36</v>
       </c>
@@ -1912,17 +1922,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H10"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5:N10 L10:M10 I5:I10 K5:K10 J5:J6 J8 J10" xr:uid="{00000000-0002-0000-0100-000000000000}">

</xml_diff>